<commit_message>
criação da função para confirmar procedimentos e identificação dos campos respectivos desse processo
</commit_message>
<xml_diff>
--- a/BASE_GUIAS_IPASGO_10-2024tTEST.xlsx
+++ b/BASE_GUIAS_IPASGO_10-2024tTEST.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b79dee6c08fdf788/Área de Trabalho/Verificação_prodecimento_ipasgo/automacao_verificacao_de_consulta_ipasgo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SUPERVISÃO ADM\Desktop\RPA_verificação_ipasgo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="11_75E9A91E134A98DEE54878D6425DCE3AC74C0377" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0A32F5E-B3DA-4EF7-B035-603400A76EC4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B060A652-588D-4F70-B536-B8A2D088B4C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="154">
   <si>
     <t>PACIENTE</t>
   </si>
@@ -58,6 +58,9 @@
     <t>QTDEATENDIMENTOS</t>
   </si>
   <si>
+    <t>QT_CONFIRMADA</t>
+  </si>
+  <si>
     <t>ERRO</t>
   </si>
   <si>
@@ -88,12 +91,18 @@
     <t>ANA CLARA TAVARES MARQUES</t>
   </si>
   <si>
+    <t>Confirmado 17/10/2024; Confirmado 17/10/2024; Confirmado 31/10/2024; Confirmado 31/10/2024; Não confirmado; Não confirmado; Não confirmado; Não confirmado</t>
+  </si>
+  <si>
     <t>ANDRE NEVES JACOB</t>
   </si>
   <si>
     <t>ANGELINA SOUZA NOGUEIRA</t>
   </si>
   <si>
+    <t>Confirmado 07/10/2024; Confirmado 07/10/2024; Confirmado 21/10/2024; Confirmado 21/10/2024; Confirmado 28/10/2024; Confirmado 28/10/2024; Confirmado 04/11/2024; Confirmado 04/11/2024</t>
+  </si>
+  <si>
     <t>ANNA CLARA BUENO DO CARMO</t>
   </si>
   <si>
@@ -473,9 +482,6 @@
   </si>
   <si>
     <t>Em análise</t>
-  </si>
-  <si>
-    <t>Qt_Confirmada</t>
   </si>
 </sst>
 </file>
@@ -844,19 +850,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" customWidth="1"/>
-    <col min="2" max="6" width="25.42578125" customWidth="1"/>
-    <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="25.7109375" customWidth="1"/>
-    <col min="9" max="9" width="33.5703125" customWidth="1"/>
-    <col min="10" max="10" width="28" customWidth="1"/>
-    <col min="12" max="12" width="32.28515625" customWidth="1"/>
+    <col min="1" max="13" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -897,18 +897,18 @@
         <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>151</v>
+        <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2">
         <v>7790108</v>
@@ -917,7 +917,7 @@
         <v>7790108155</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E2" s="2">
         <v>45559</v>
@@ -947,12 +947,12 @@
         <v>1</v>
       </c>
       <c r="O2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B3">
         <v>7792026</v>
@@ -961,7 +961,7 @@
         <v>7792026148</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E3" s="2">
         <v>45559</v>
@@ -993,7 +993,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B4">
         <v>7792797</v>
@@ -1002,7 +1002,7 @@
         <v>7792797172</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E4" s="2">
         <v>45559</v>
@@ -1034,7 +1034,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B5">
         <v>7793039</v>
@@ -1043,7 +1043,7 @@
         <v>7793039187</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E5" s="2">
         <v>45559</v>
@@ -1075,7 +1075,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6">
         <v>7795445</v>
@@ -1084,7 +1084,7 @@
         <v>7795445126</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E6" s="2">
         <v>45559</v>
@@ -1116,7 +1116,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B7">
         <v>7795650</v>
@@ -1125,7 +1125,7 @@
         <v>7795650176</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E7" s="2">
         <v>45559</v>
@@ -1157,7 +1157,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B8">
         <v>7795741</v>
@@ -1166,7 +1166,7 @@
         <v>7795741144</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E8" s="2">
         <v>45559</v>
@@ -1198,7 +1198,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B9">
         <v>7795804</v>
@@ -1207,7 +1207,7 @@
         <v>7795804150</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E9" s="2">
         <v>45559</v>
@@ -1239,7 +1239,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B10">
         <v>7796079</v>
@@ -1248,7 +1248,7 @@
         <v>7796079394</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E10" s="2">
         <v>45559</v>
@@ -1272,15 +1272,18 @@
         <v>4115</v>
       </c>
       <c r="L10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M10">
         <v>1</v>
+      </c>
+      <c r="O10" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B11">
         <v>7801500</v>
@@ -1289,7 +1292,7 @@
         <v>7801500152</v>
       </c>
       <c r="D11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E11" s="2">
         <v>45559</v>
@@ -1321,7 +1324,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B12">
         <v>7801570</v>
@@ -1330,7 +1333,7 @@
         <v>7801570185</v>
       </c>
       <c r="D12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E12" s="2">
         <v>45559</v>
@@ -1359,10 +1362,13 @@
       <c r="M12">
         <v>1</v>
       </c>
+      <c r="O12" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B13">
         <v>7801602</v>
@@ -1371,7 +1377,7 @@
         <v>7801602156</v>
       </c>
       <c r="D13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E13" s="2">
         <v>45559</v>
@@ -1403,7 +1409,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B14">
         <v>7801643</v>
@@ -1412,7 +1418,7 @@
         <v>7801643162</v>
       </c>
       <c r="D14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E14" s="2">
         <v>45559</v>
@@ -1444,7 +1450,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B15">
         <v>7801692</v>
@@ -1453,7 +1459,7 @@
         <v>7801692349</v>
       </c>
       <c r="D15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E15" s="2">
         <v>45559</v>
@@ -1485,7 +1491,7 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B16">
         <v>7801736</v>
@@ -1494,7 +1500,7 @@
         <v>7801736162</v>
       </c>
       <c r="D16" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E16" s="2">
         <v>45559</v>
@@ -1526,7 +1532,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B17">
         <v>7801774</v>
@@ -1535,7 +1541,7 @@
         <v>7801774191</v>
       </c>
       <c r="D17" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E17" s="2">
         <v>45559</v>
@@ -1567,7 +1573,7 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B18">
         <v>7802015</v>
@@ -1576,7 +1582,7 @@
         <v>7802015180</v>
       </c>
       <c r="D18" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E18" s="2">
         <v>45559</v>
@@ -1608,7 +1614,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B19">
         <v>7802073</v>
@@ -1617,7 +1623,7 @@
         <v>7802073154</v>
       </c>
       <c r="D19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E19" s="2">
         <v>45559</v>
@@ -1649,7 +1655,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B20">
         <v>7808586</v>
@@ -1658,7 +1664,7 @@
         <v>7808586169</v>
       </c>
       <c r="D20" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E20" s="2">
         <v>45559</v>
@@ -1690,7 +1696,7 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B21">
         <v>7808678</v>
@@ -1699,7 +1705,7 @@
         <v>7808678166</v>
       </c>
       <c r="D21" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E21" s="2">
         <v>45559</v>
@@ -1731,7 +1737,7 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B22">
         <v>7808766</v>
@@ -1740,7 +1746,7 @@
         <v>7808766197</v>
       </c>
       <c r="D22" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E22" s="2">
         <v>45559</v>
@@ -1772,7 +1778,7 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B23">
         <v>7808834</v>
@@ -1781,7 +1787,7 @@
         <v>7808834165</v>
       </c>
       <c r="D23" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E23" s="2">
         <v>45559</v>
@@ -1807,7 +1813,7 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B24">
         <v>7808924</v>
@@ -1816,7 +1822,7 @@
         <v>7808924136</v>
       </c>
       <c r="D24" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E24" s="2">
         <v>45559</v>
@@ -1848,7 +1854,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B25">
         <v>7809073</v>
@@ -1857,7 +1863,7 @@
         <v>7809073121</v>
       </c>
       <c r="D25" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E25" s="2">
         <v>45559</v>
@@ -1889,7 +1895,7 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B26">
         <v>7809144</v>
@@ -1898,7 +1904,7 @@
         <v>7809144184</v>
       </c>
       <c r="D26" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E26" s="2">
         <v>45559</v>
@@ -1930,7 +1936,7 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B27">
         <v>7809214</v>
@@ -1939,7 +1945,7 @@
         <v>7809214176</v>
       </c>
       <c r="D27" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E27" s="2">
         <v>45559</v>
@@ -1971,7 +1977,7 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B28">
         <v>7809285</v>
@@ -1980,7 +1986,7 @@
         <v>7809285114</v>
       </c>
       <c r="D28" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E28" s="2">
         <v>45559</v>
@@ -2012,7 +2018,7 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B29">
         <v>7809377</v>
@@ -2021,7 +2027,7 @@
         <v>7809377123</v>
       </c>
       <c r="D29" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E29" s="2">
         <v>45559</v>
@@ -2053,7 +2059,7 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B30">
         <v>7812426</v>
@@ -2062,7 +2068,7 @@
         <v>7812426117</v>
       </c>
       <c r="D30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E30" s="2">
         <v>45559</v>
@@ -2094,7 +2100,7 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B31">
         <v>7814092</v>
@@ -2103,7 +2109,7 @@
         <v>7814092121</v>
       </c>
       <c r="D31" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E31" s="2">
         <v>45559</v>
@@ -2135,7 +2141,7 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B32">
         <v>7814390</v>
@@ -2144,7 +2150,7 @@
         <v>7814390161</v>
       </c>
       <c r="D32" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E32" s="2">
         <v>45559</v>
@@ -2176,7 +2182,7 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B33">
         <v>7814445</v>
@@ -2185,7 +2191,7 @@
         <v>7814445165</v>
       </c>
       <c r="D33" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E33" s="2">
         <v>45559</v>
@@ -2217,7 +2223,7 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B34">
         <v>7814484</v>
@@ -2226,7 +2232,7 @@
         <v>7814484109</v>
       </c>
       <c r="D34" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E34" s="2">
         <v>45559</v>
@@ -2258,7 +2264,7 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B35">
         <v>7860299</v>
@@ -2267,7 +2273,7 @@
         <v>7860299362</v>
       </c>
       <c r="D35" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E35" s="2">
         <v>45561</v>
@@ -2299,7 +2305,7 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B36">
         <v>7860895</v>
@@ -2308,7 +2314,7 @@
         <v>7860895119</v>
       </c>
       <c r="D36" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E36" s="2">
         <v>45561</v>
@@ -2340,7 +2346,7 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B37">
         <v>7860947</v>
@@ -2349,7 +2355,7 @@
         <v>7860947161</v>
       </c>
       <c r="D37" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E37" s="2">
         <v>45561</v>
@@ -2381,7 +2387,7 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B38">
         <v>7865936</v>
@@ -2390,7 +2396,7 @@
         <v>7865936189</v>
       </c>
       <c r="D38" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E38" s="2">
         <v>45561</v>
@@ -2422,7 +2428,7 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B39">
         <v>7870383</v>
@@ -2431,7 +2437,7 @@
         <v>7870383116</v>
       </c>
       <c r="D39" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E39" s="2">
         <v>45561</v>
@@ -2463,7 +2469,7 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B40">
         <v>7870465</v>
@@ -2472,7 +2478,7 @@
         <v>7870465161</v>
       </c>
       <c r="D40" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E40" s="2">
         <v>45561</v>
@@ -2504,7 +2510,7 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B41">
         <v>7871329</v>
@@ -2513,7 +2519,7 @@
         <v>7871329166</v>
       </c>
       <c r="D41" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E41" s="2">
         <v>45561</v>
@@ -2545,7 +2551,7 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B42">
         <v>7871681</v>
@@ -2554,7 +2560,7 @@
         <v>7871681104</v>
       </c>
       <c r="D42" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E42" s="2">
         <v>45561</v>
@@ -2586,7 +2592,7 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B43">
         <v>7871763</v>
@@ -2595,7 +2601,7 @@
         <v>7871763180</v>
       </c>
       <c r="D43" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E43" s="2">
         <v>45561</v>
@@ -2627,7 +2633,7 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B44">
         <v>7871837</v>
@@ -2636,7 +2642,7 @@
         <v>7871837154</v>
       </c>
       <c r="D44" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E44" s="2">
         <v>45561</v>
@@ -2668,7 +2674,7 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B45">
         <v>7871984</v>
@@ -2677,7 +2683,7 @@
         <v>7871984189</v>
       </c>
       <c r="D45" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E45" s="2">
         <v>45561</v>
@@ -2709,7 +2715,7 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B46">
         <v>7872034</v>
@@ -2718,7 +2724,7 @@
         <v>7872034151</v>
       </c>
       <c r="D46" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E46" s="2">
         <v>45561</v>
@@ -2750,7 +2756,7 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B47">
         <v>7872184</v>
@@ -2759,7 +2765,7 @@
         <v>7872184179</v>
       </c>
       <c r="D47" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E47" s="2">
         <v>45561</v>
@@ -2791,7 +2797,7 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B48">
         <v>7872281</v>
@@ -2800,7 +2806,7 @@
         <v>7872281188</v>
       </c>
       <c r="D48" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E48" s="2">
         <v>45561</v>
@@ -2832,7 +2838,7 @@
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B49">
         <v>7872396</v>
@@ -2841,7 +2847,7 @@
         <v>7872396106</v>
       </c>
       <c r="D49" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E49" s="2">
         <v>45561</v>
@@ -2873,7 +2879,7 @@
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B50">
         <v>7872467</v>
@@ -2882,7 +2888,7 @@
         <v>7872467193</v>
       </c>
       <c r="D50" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E50" s="2">
         <v>45561</v>
@@ -2914,7 +2920,7 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B51">
         <v>7872549</v>
@@ -2923,7 +2929,7 @@
         <v>7872549188</v>
       </c>
       <c r="D51" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E51" s="2">
         <v>45561</v>
@@ -2955,7 +2961,7 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B52">
         <v>7874829</v>
@@ -2964,7 +2970,7 @@
         <v>7874829109</v>
       </c>
       <c r="D52" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E52" s="2">
         <v>45561</v>
@@ -2996,7 +3002,7 @@
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B53">
         <v>7875277</v>
@@ -3005,7 +3011,7 @@
         <v>7875277143</v>
       </c>
       <c r="D53" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E53" s="2">
         <v>45561</v>
@@ -3037,7 +3043,7 @@
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B54">
         <v>7875462</v>
@@ -3046,7 +3052,7 @@
         <v>7875462158</v>
       </c>
       <c r="D54" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E54" s="2">
         <v>45561</v>
@@ -3078,7 +3084,7 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B55">
         <v>7876032</v>
@@ -3087,7 +3093,7 @@
         <v>7876032152</v>
       </c>
       <c r="D55" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E55" s="2">
         <v>45561</v>
@@ -3119,7 +3125,7 @@
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B56">
         <v>7876433</v>
@@ -3128,7 +3134,7 @@
         <v>7876433142</v>
       </c>
       <c r="D56" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E56" s="2">
         <v>45561</v>
@@ -3160,7 +3166,7 @@
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B57">
         <v>7876594</v>
@@ -3169,7 +3175,7 @@
         <v>7876594180</v>
       </c>
       <c r="D57" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E57" s="2">
         <v>45561</v>
@@ -3201,7 +3207,7 @@
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B58">
         <v>7876714</v>
@@ -3210,7 +3216,7 @@
         <v>7876714112</v>
       </c>
       <c r="D58" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E58" s="2">
         <v>45561</v>
@@ -3242,7 +3248,7 @@
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B59">
         <v>7876939</v>
@@ -3251,7 +3257,7 @@
         <v>7876939372</v>
       </c>
       <c r="D59" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E59" s="2">
         <v>45561</v>
@@ -3283,7 +3289,7 @@
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B60">
         <v>7877604</v>
@@ -3292,7 +3298,7 @@
         <v>7877604306</v>
       </c>
       <c r="D60" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E60" s="2">
         <v>45561</v>
@@ -3324,7 +3330,7 @@
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B61">
         <v>7877713</v>
@@ -3333,7 +3339,7 @@
         <v>7877713336</v>
       </c>
       <c r="D61" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E61" s="2">
         <v>45561</v>
@@ -3365,7 +3371,7 @@
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B62">
         <v>7877931</v>
@@ -3374,7 +3380,7 @@
         <v>7877931179</v>
       </c>
       <c r="D62" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E62" s="2">
         <v>45561</v>
@@ -3406,7 +3412,7 @@
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B63">
         <v>7878098</v>
@@ -3415,7 +3421,7 @@
         <v>7878098192</v>
       </c>
       <c r="D63" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E63" s="2">
         <v>45561</v>
@@ -3447,7 +3453,7 @@
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B64">
         <v>7878246</v>
@@ -3456,7 +3462,7 @@
         <v>7878246140</v>
       </c>
       <c r="D64" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E64" s="2">
         <v>45561</v>
@@ -3488,7 +3494,7 @@
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B65">
         <v>7879005</v>
@@ -3497,7 +3503,7 @@
         <v>7879005163</v>
       </c>
       <c r="D65" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E65" s="2">
         <v>45561</v>
@@ -3529,7 +3535,7 @@
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B66">
         <v>7879105</v>
@@ -3538,7 +3544,7 @@
         <v>7879105103</v>
       </c>
       <c r="D66" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E66" s="2">
         <v>45561</v>
@@ -3570,7 +3576,7 @@
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B67">
         <v>7879350</v>
@@ -3579,7 +3585,7 @@
         <v>7879350122</v>
       </c>
       <c r="D67" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E67" s="2">
         <v>45561</v>
@@ -3611,7 +3617,7 @@
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B68">
         <v>7879419</v>
@@ -3620,7 +3626,7 @@
         <v>7879419129</v>
       </c>
       <c r="D68" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E68" s="2">
         <v>45561</v>
@@ -3652,7 +3658,7 @@
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B69">
         <v>7879492</v>
@@ -3661,7 +3667,7 @@
         <v>7879492172</v>
       </c>
       <c r="D69" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E69" s="2">
         <v>45561</v>
@@ -3693,7 +3699,7 @@
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B70">
         <v>7879573</v>
@@ -3702,7 +3708,7 @@
         <v>7879573195</v>
       </c>
       <c r="D70" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E70" s="2">
         <v>45561</v>
@@ -3734,7 +3740,7 @@
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B71">
         <v>7879669</v>
@@ -3743,7 +3749,7 @@
         <v>7879669356</v>
       </c>
       <c r="D71" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E71" s="2">
         <v>45561</v>
@@ -3775,7 +3781,7 @@
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B72">
         <v>7880295</v>
@@ -3784,7 +3790,7 @@
         <v>7880295194</v>
       </c>
       <c r="D72" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E72" s="2">
         <v>45561</v>
@@ -3816,7 +3822,7 @@
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B73">
         <v>7880431</v>
@@ -3825,7 +3831,7 @@
         <v>7880431106</v>
       </c>
       <c r="D73" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E73" s="2">
         <v>45561</v>
@@ -3857,7 +3863,7 @@
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B74">
         <v>7881246</v>
@@ -3866,7 +3872,7 @@
         <v>7881246116</v>
       </c>
       <c r="D74" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E74" s="2">
         <v>45561</v>
@@ -3898,7 +3904,7 @@
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B75">
         <v>7881361</v>
@@ -3907,7 +3913,7 @@
         <v>7881361180</v>
       </c>
       <c r="D75" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E75" s="2">
         <v>45561</v>
@@ -3939,7 +3945,7 @@
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B76">
         <v>7881532</v>
@@ -3948,7 +3954,7 @@
         <v>7881532160</v>
       </c>
       <c r="D76" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E76" s="2">
         <v>45561</v>
@@ -3980,7 +3986,7 @@
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B77">
         <v>7881650</v>
@@ -3989,7 +3995,7 @@
         <v>7881650176</v>
       </c>
       <c r="D77" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E77" s="2">
         <v>45561</v>
@@ -4021,7 +4027,7 @@
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B78">
         <v>7881690</v>
@@ -4030,7 +4036,7 @@
         <v>7881690173</v>
       </c>
       <c r="D78" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E78" s="2">
         <v>45561</v>
@@ -4062,7 +4068,7 @@
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B79">
         <v>7881710</v>
@@ -4071,7 +4077,7 @@
         <v>7881710115</v>
       </c>
       <c r="D79" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E79" s="2">
         <v>45561</v>
@@ -4103,7 +4109,7 @@
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B80">
         <v>7881850</v>
@@ -4112,7 +4118,7 @@
         <v>7881850168</v>
       </c>
       <c r="D80" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E80" s="2">
         <v>45561</v>
@@ -4144,7 +4150,7 @@
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B81">
         <v>7881933</v>
@@ -4153,7 +4159,7 @@
         <v>7881933333</v>
       </c>
       <c r="D81" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E81" s="2">
         <v>45561</v>
@@ -4185,7 +4191,7 @@
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B82">
         <v>7882032</v>
@@ -4194,7 +4200,7 @@
         <v>7882032196</v>
       </c>
       <c r="D82" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E82" s="2">
         <v>45561</v>
@@ -4226,7 +4232,7 @@
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B83">
         <v>7882128</v>
@@ -4235,7 +4241,7 @@
         <v>7882128191</v>
       </c>
       <c r="D83" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E83" s="2">
         <v>45561</v>
@@ -4267,7 +4273,7 @@
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B84">
         <v>7882132</v>
@@ -4276,7 +4282,7 @@
         <v>7882132168</v>
       </c>
       <c r="D84" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E84" s="2">
         <v>45561</v>
@@ -4308,7 +4314,7 @@
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B85">
         <v>7882236</v>
@@ -4317,7 +4323,7 @@
         <v>7882236106</v>
       </c>
       <c r="D85" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E85" s="2">
         <v>45561</v>
@@ -4349,7 +4355,7 @@
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B86">
         <v>7882241</v>
@@ -4358,7 +4364,7 @@
         <v>7882241192</v>
       </c>
       <c r="D86" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E86" s="2">
         <v>45561</v>
@@ -4390,7 +4396,7 @@
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B87">
         <v>7882384</v>
@@ -4399,7 +4405,7 @@
         <v>7882384196</v>
       </c>
       <c r="D87" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E87" s="2">
         <v>45561</v>
@@ -4431,7 +4437,7 @@
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B88">
         <v>7882444</v>
@@ -4440,7 +4446,7 @@
         <v>7882444362</v>
       </c>
       <c r="D88" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E88" s="2">
         <v>45561</v>
@@ -4472,7 +4478,7 @@
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B89">
         <v>7882563</v>
@@ -4481,7 +4487,7 @@
         <v>7882563124</v>
       </c>
       <c r="D89" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E89" s="2">
         <v>45561</v>
@@ -4513,7 +4519,7 @@
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B90">
         <v>7882600</v>
@@ -4522,7 +4528,7 @@
         <v>7882600335</v>
       </c>
       <c r="D90" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E90" s="2">
         <v>45561</v>
@@ -4554,7 +4560,7 @@
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B91">
         <v>7882607</v>
@@ -4563,7 +4569,7 @@
         <v>7882607392</v>
       </c>
       <c r="D91" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E91" s="2">
         <v>45561</v>
@@ -4595,7 +4601,7 @@
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B92">
         <v>7882657</v>
@@ -4604,7 +4610,7 @@
         <v>7882657306</v>
       </c>
       <c r="D92" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E92" s="2">
         <v>45561</v>
@@ -4636,7 +4642,7 @@
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B93">
         <v>7882661</v>
@@ -4645,7 +4651,7 @@
         <v>7882661100</v>
       </c>
       <c r="D93" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E93" s="2">
         <v>45561</v>
@@ -4677,7 +4683,7 @@
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B94">
         <v>7882708</v>
@@ -4686,7 +4692,7 @@
         <v>7882708351</v>
       </c>
       <c r="D94" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E94" s="2">
         <v>45561</v>
@@ -4718,7 +4724,7 @@
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B95">
         <v>7882710</v>
@@ -4727,7 +4733,7 @@
         <v>7882710180</v>
       </c>
       <c r="D95" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E95" s="2">
         <v>45561</v>
@@ -4759,7 +4765,7 @@
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B96">
         <v>7882970</v>
@@ -4768,7 +4774,7 @@
         <v>7882970124</v>
       </c>
       <c r="D96" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E96" s="2">
         <v>45561</v>
@@ -4800,7 +4806,7 @@
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B97">
         <v>7882971</v>
@@ -4809,7 +4815,7 @@
         <v>7882971125</v>
       </c>
       <c r="D97" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E97" s="2">
         <v>45561</v>
@@ -4841,7 +4847,7 @@
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B98">
         <v>7883063</v>
@@ -4850,7 +4856,7 @@
         <v>7883063162</v>
       </c>
       <c r="D98" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E98" s="2">
         <v>45561</v>
@@ -4882,7 +4888,7 @@
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B99">
         <v>7883081</v>
@@ -4891,7 +4897,7 @@
         <v>7883081110</v>
       </c>
       <c r="D99" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E99" s="2">
         <v>45561</v>
@@ -4923,7 +4929,7 @@
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B100">
         <v>7883164</v>
@@ -4932,7 +4938,7 @@
         <v>7883164375</v>
       </c>
       <c r="D100" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E100" s="2">
         <v>45561</v>
@@ -4964,7 +4970,7 @@
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B101">
         <v>7883182</v>
@@ -4973,7 +4979,7 @@
         <v>7883182125</v>
       </c>
       <c r="D101" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E101" s="2">
         <v>45561</v>
@@ -5005,7 +5011,7 @@
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B102">
         <v>7883637</v>
@@ -5014,7 +5020,7 @@
         <v>7883637125</v>
       </c>
       <c r="D102" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E102" s="2">
         <v>45561</v>
@@ -5046,7 +5052,7 @@
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B103">
         <v>7883675</v>
@@ -5055,7 +5061,7 @@
         <v>7883675128</v>
       </c>
       <c r="D103" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E103" s="2">
         <v>45561</v>
@@ -5087,7 +5093,7 @@
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B104">
         <v>7883699</v>
@@ -5096,7 +5102,7 @@
         <v>7883699138</v>
       </c>
       <c r="D104" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E104" s="2">
         <v>45561</v>
@@ -5128,7 +5134,7 @@
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B105">
         <v>7920440</v>
@@ -5137,7 +5143,7 @@
         <v>7920440375</v>
       </c>
       <c r="D105" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E105" s="2">
         <v>45563</v>
@@ -5169,7 +5175,7 @@
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B106">
         <v>7920446</v>
@@ -5178,7 +5184,7 @@
         <v>7920446381</v>
       </c>
       <c r="D106" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E106" s="2">
         <v>45563</v>
@@ -5210,7 +5216,7 @@
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B107">
         <v>7920453</v>
@@ -5219,7 +5225,7 @@
         <v>7920453163</v>
       </c>
       <c r="D107" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E107" s="2">
         <v>45563</v>
@@ -5251,7 +5257,7 @@
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B108">
         <v>7920457</v>
@@ -5260,7 +5266,7 @@
         <v>7920457191</v>
       </c>
       <c r="D108" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E108" s="2">
         <v>45563</v>
@@ -5292,7 +5298,7 @@
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B109">
         <v>7920478</v>
@@ -5301,7 +5307,7 @@
         <v>7920478147</v>
       </c>
       <c r="D109" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E109" s="2">
         <v>45563</v>
@@ -5333,7 +5339,7 @@
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B110">
         <v>7920485</v>
@@ -5342,7 +5348,7 @@
         <v>7920485363</v>
       </c>
       <c r="D110" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E110" s="2">
         <v>45563</v>
@@ -5374,7 +5380,7 @@
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B111">
         <v>7920491</v>
@@ -5383,7 +5389,7 @@
         <v>7920491112</v>
       </c>
       <c r="D111" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E111" s="2">
         <v>45563</v>
@@ -5415,7 +5421,7 @@
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B112">
         <v>7920546</v>
@@ -5424,7 +5430,7 @@
         <v>7920546151</v>
       </c>
       <c r="D112" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E112" s="2">
         <v>45563</v>
@@ -5456,7 +5462,7 @@
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B113">
         <v>7920553</v>
@@ -5465,7 +5471,7 @@
         <v>7920553111</v>
       </c>
       <c r="D113" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E113" s="2">
         <v>45563</v>
@@ -5497,7 +5503,7 @@
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B114">
         <v>7920558</v>
@@ -5506,7 +5512,7 @@
         <v>7920558152</v>
       </c>
       <c r="D114" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E114" s="2">
         <v>45563</v>
@@ -5538,7 +5544,7 @@
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B115">
         <v>7920565</v>
@@ -5547,7 +5553,7 @@
         <v>7920565143</v>
       </c>
       <c r="D115" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E115" s="2">
         <v>45563</v>
@@ -5579,7 +5585,7 @@
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B116">
         <v>7920574</v>
@@ -5588,7 +5594,7 @@
         <v>7920574155</v>
       </c>
       <c r="D116" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E116" s="2">
         <v>45563</v>
@@ -5620,7 +5626,7 @@
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B117">
         <v>7920590</v>
@@ -5629,7 +5635,7 @@
         <v>7920590145</v>
       </c>
       <c r="D117" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E117" s="2">
         <v>45563</v>
@@ -5661,7 +5667,7 @@
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B118">
         <v>7920593</v>
@@ -5670,7 +5676,7 @@
         <v>7920593194</v>
       </c>
       <c r="D118" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E118" s="2">
         <v>45563</v>
@@ -5702,7 +5708,7 @@
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B119">
         <v>7920595</v>
@@ -5711,7 +5717,7 @@
         <v>7920595136</v>
       </c>
       <c r="D119" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E119" s="2">
         <v>45563</v>
@@ -5743,7 +5749,7 @@
     </row>
     <row r="120" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B120">
         <v>7920604</v>
@@ -5752,7 +5758,7 @@
         <v>7920604140</v>
       </c>
       <c r="D120" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E120" s="2">
         <v>45563</v>
@@ -5784,7 +5790,7 @@
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B121">
         <v>7920622</v>
@@ -5793,7 +5799,7 @@
         <v>7920622125</v>
       </c>
       <c r="D121" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E121" s="2">
         <v>45563</v>
@@ -5825,7 +5831,7 @@
     </row>
     <row r="122" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B122">
         <v>7920628</v>
@@ -5834,7 +5840,7 @@
         <v>7920628305</v>
       </c>
       <c r="D122" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E122" s="2">
         <v>45563</v>
@@ -5866,7 +5872,7 @@
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B123">
         <v>7920634</v>
@@ -5875,7 +5881,7 @@
         <v>7920634186</v>
       </c>
       <c r="D123" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E123" s="2">
         <v>45563</v>
@@ -5907,7 +5913,7 @@
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B124">
         <v>7920637</v>
@@ -5916,7 +5922,7 @@
         <v>7920637145</v>
       </c>
       <c r="D124" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E124" s="2">
         <v>45563</v>
@@ -5948,7 +5954,7 @@
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B125">
         <v>7920644</v>
@@ -5957,7 +5963,7 @@
         <v>7920644131</v>
       </c>
       <c r="D125" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E125" s="2">
         <v>45563</v>
@@ -5989,7 +5995,7 @@
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B126">
         <v>7920650</v>
@@ -5998,7 +6004,7 @@
         <v>7920650182</v>
       </c>
       <c r="D126" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E126" s="2">
         <v>45563</v>
@@ -6030,7 +6036,7 @@
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B127">
         <v>7920653</v>
@@ -6039,7 +6045,7 @@
         <v>7920653145</v>
       </c>
       <c r="D127" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E127" s="2">
         <v>45563</v>
@@ -6071,7 +6077,7 @@
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B128">
         <v>7920657</v>
@@ -6080,7 +6086,7 @@
         <v>7920657197</v>
       </c>
       <c r="D128" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E128" s="2">
         <v>45563</v>
@@ -6112,7 +6118,7 @@
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B129">
         <v>7920662</v>
@@ -6121,7 +6127,7 @@
         <v>7920662118</v>
       </c>
       <c r="D129" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E129" s="2">
         <v>45563</v>
@@ -6153,7 +6159,7 @@
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B130">
         <v>7920677</v>
@@ -6162,7 +6168,7 @@
         <v>7920677170</v>
       </c>
       <c r="D130" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E130" s="2">
         <v>45563</v>
@@ -6194,7 +6200,7 @@
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B131">
         <v>7920680</v>
@@ -6203,7 +6209,7 @@
         <v>7920680186</v>
       </c>
       <c r="D131" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E131" s="2">
         <v>45563</v>
@@ -6235,7 +6241,7 @@
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B132">
         <v>7920689</v>
@@ -6244,7 +6250,7 @@
         <v>7920689131</v>
       </c>
       <c r="D132" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E132" s="2">
         <v>45563</v>
@@ -6276,7 +6282,7 @@
     </row>
     <row r="133" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B133">
         <v>7920711</v>
@@ -6285,7 +6291,7 @@
         <v>7920711128</v>
       </c>
       <c r="D133" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E133" s="2">
         <v>45563</v>
@@ -6317,7 +6323,7 @@
     </row>
     <row r="134" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B134">
         <v>7920718</v>
@@ -6326,7 +6332,7 @@
         <v>7920718121</v>
       </c>
       <c r="D134" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E134" s="2">
         <v>45563</v>
@@ -6358,7 +6364,7 @@
     </row>
     <row r="135" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B135">
         <v>7920722</v>
@@ -6367,7 +6373,7 @@
         <v>7920722189</v>
       </c>
       <c r="D135" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E135" s="2">
         <v>45563</v>
@@ -6393,7 +6399,7 @@
     </row>
     <row r="136" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B136">
         <v>7920734</v>
@@ -6402,7 +6408,7 @@
         <v>7920734392</v>
       </c>
       <c r="D136" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E136" s="2">
         <v>45563</v>
@@ -6434,7 +6440,7 @@
     </row>
     <row r="137" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B137">
         <v>7920775</v>
@@ -6443,7 +6449,7 @@
         <v>7920775374</v>
       </c>
       <c r="D137" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E137" s="2">
         <v>45563</v>
@@ -6475,7 +6481,7 @@
     </row>
     <row r="138" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B138">
         <v>7920778</v>
@@ -6484,7 +6490,7 @@
         <v>7920778327</v>
       </c>
       <c r="D138" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E138" s="2">
         <v>45563</v>
@@ -6516,7 +6522,7 @@
     </row>
     <row r="139" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B139">
         <v>7920785</v>
@@ -6525,7 +6531,7 @@
         <v>7920785171</v>
       </c>
       <c r="D139" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E139" s="2">
         <v>45563</v>
@@ -6557,7 +6563,7 @@
     </row>
     <row r="140" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B140">
         <v>7920788</v>
@@ -6566,7 +6572,7 @@
         <v>7920788154</v>
       </c>
       <c r="D140" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E140" s="2">
         <v>45563</v>
@@ -6598,7 +6604,7 @@
     </row>
     <row r="141" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B141">
         <v>7920794</v>
@@ -6607,7 +6613,7 @@
         <v>7920794119</v>
       </c>
       <c r="D141" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E141" s="2">
         <v>45563</v>
@@ -6639,7 +6645,7 @@
     </row>
     <row r="142" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B142">
         <v>7920799</v>
@@ -6648,7 +6654,7 @@
         <v>7920799142</v>
       </c>
       <c r="D142" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E142" s="2">
         <v>45563</v>
@@ -6680,7 +6686,7 @@
     </row>
     <row r="143" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B143">
         <v>7920804</v>
@@ -6689,7 +6695,7 @@
         <v>7920804152</v>
       </c>
       <c r="D143" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E143" s="2">
         <v>45563</v>
@@ -6721,7 +6727,7 @@
     </row>
     <row r="144" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B144">
         <v>7920807</v>
@@ -6730,7 +6736,7 @@
         <v>7920807107</v>
       </c>
       <c r="D144" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E144" s="2">
         <v>45563</v>
@@ -6762,7 +6768,7 @@
     </row>
     <row r="145" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B145">
         <v>7920810</v>
@@ -6771,7 +6777,7 @@
         <v>7920810165</v>
       </c>
       <c r="D145" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E145" s="2">
         <v>45563</v>
@@ -6803,7 +6809,7 @@
     </row>
     <row r="146" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B146">
         <v>7920824</v>
@@ -6812,7 +6818,7 @@
         <v>7920824111</v>
       </c>
       <c r="D146" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E146" s="2">
         <v>45563</v>
@@ -6844,7 +6850,7 @@
     </row>
     <row r="147" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B147">
         <v>7920828</v>
@@ -6853,7 +6859,7 @@
         <v>7920828345</v>
       </c>
       <c r="D147" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E147" s="2">
         <v>45563</v>
@@ -6879,7 +6885,7 @@
     </row>
     <row r="148" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B148">
         <v>7920841</v>
@@ -6888,7 +6894,7 @@
         <v>7920841348</v>
       </c>
       <c r="D148" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E148" s="2">
         <v>45563</v>
@@ -6920,7 +6926,7 @@
     </row>
     <row r="149" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B149">
         <v>7920845</v>
@@ -6929,7 +6935,7 @@
         <v>7920845324</v>
       </c>
       <c r="D149" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E149" s="2">
         <v>45563</v>
@@ -6961,7 +6967,7 @@
     </row>
     <row r="150" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B150">
         <v>7920852</v>
@@ -6970,7 +6976,7 @@
         <v>7920852322</v>
       </c>
       <c r="D150" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E150" s="2">
         <v>45563</v>
@@ -7002,7 +7008,7 @@
     </row>
     <row r="151" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B151">
         <v>7920856</v>
@@ -7011,7 +7017,7 @@
         <v>7920856306</v>
       </c>
       <c r="D151" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E151" s="2">
         <v>45563</v>
@@ -7043,7 +7049,7 @@
     </row>
     <row r="152" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B152">
         <v>7920862</v>
@@ -7052,7 +7058,7 @@
         <v>7920862324</v>
       </c>
       <c r="D152" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E152" s="2">
         <v>45563</v>
@@ -7084,7 +7090,7 @@
     </row>
     <row r="153" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B153">
         <v>7940877</v>
@@ -7093,7 +7099,7 @@
         <v>7940877156</v>
       </c>
       <c r="D153" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E153" s="2">
         <v>45565</v>
@@ -7125,7 +7131,7 @@
     </row>
     <row r="154" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B154">
         <v>7940949</v>
@@ -7134,7 +7140,7 @@
         <v>7940949104</v>
       </c>
       <c r="D154" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E154" s="2">
         <v>45565</v>
@@ -7166,7 +7172,7 @@
     </row>
     <row r="155" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B155">
         <v>7941147</v>
@@ -7175,7 +7181,7 @@
         <v>7941147178</v>
       </c>
       <c r="D155" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E155" s="2">
         <v>45565</v>
@@ -7207,7 +7213,7 @@
     </row>
     <row r="156" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B156">
         <v>7941784</v>
@@ -7216,7 +7222,7 @@
         <v>7941784391</v>
       </c>
       <c r="D156" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E156" s="2">
         <v>45565</v>
@@ -7248,7 +7254,7 @@
     </row>
     <row r="157" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B157">
         <v>7941934</v>
@@ -7257,7 +7263,7 @@
         <v>7941934173</v>
       </c>
       <c r="D157" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E157" s="2">
         <v>45565</v>
@@ -7289,7 +7295,7 @@
     </row>
     <row r="158" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B158">
         <v>7942070</v>
@@ -7298,7 +7304,7 @@
         <v>7942070168</v>
       </c>
       <c r="D158" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E158" s="2">
         <v>45565</v>
@@ -7330,7 +7336,7 @@
     </row>
     <row r="159" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B159">
         <v>7942216</v>
@@ -7339,7 +7345,7 @@
         <v>7942216176</v>
       </c>
       <c r="D159" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E159" s="2">
         <v>45565</v>
@@ -7371,7 +7377,7 @@
     </row>
     <row r="160" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B160">
         <v>7943591</v>
@@ -7380,7 +7386,7 @@
         <v>7943591129</v>
       </c>
       <c r="D160" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E160" s="2">
         <v>45565</v>
@@ -7412,7 +7418,7 @@
     </row>
     <row r="161" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B161">
         <v>7944303</v>
@@ -7421,7 +7427,7 @@
         <v>7944303103</v>
       </c>
       <c r="D161" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E161" s="2">
         <v>45565</v>
@@ -7453,7 +7459,7 @@
     </row>
     <row r="162" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B162">
         <v>7944833</v>
@@ -7462,7 +7468,7 @@
         <v>7944833126</v>
       </c>
       <c r="D162" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E162" s="2">
         <v>45565</v>
@@ -7494,7 +7500,7 @@
     </row>
     <row r="163" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B163">
         <v>7945008</v>
@@ -7503,7 +7509,7 @@
         <v>7945008115</v>
       </c>
       <c r="D163" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E163" s="2">
         <v>45565</v>
@@ -7535,7 +7541,7 @@
     </row>
     <row r="164" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B164">
         <v>7945291</v>
@@ -7544,7 +7550,7 @@
         <v>7945291373</v>
       </c>
       <c r="D164" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E164" s="2">
         <v>45565</v>
@@ -7576,7 +7582,7 @@
     </row>
     <row r="165" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B165">
         <v>7945978</v>
@@ -7585,7 +7591,7 @@
         <v>7945978361</v>
       </c>
       <c r="D165" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E165" s="2">
         <v>45565</v>
@@ -7617,7 +7623,7 @@
     </row>
     <row r="166" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B166">
         <v>7947222</v>
@@ -7626,7 +7632,7 @@
         <v>7947222186</v>
       </c>
       <c r="D166" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E166" s="2">
         <v>45565</v>
@@ -7658,7 +7664,7 @@
     </row>
     <row r="167" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B167">
         <v>7958623</v>
@@ -7667,7 +7673,7 @@
         <v>7958623379</v>
       </c>
       <c r="D167" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E167" s="2">
         <v>45566</v>
@@ -7693,7 +7699,7 @@
     </row>
     <row r="168" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B168">
         <v>7981803</v>
@@ -7702,7 +7708,7 @@
         <v>7981803183</v>
       </c>
       <c r="D168" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E168" s="2">
         <v>45574</v>
@@ -7734,7 +7740,7 @@
     </row>
     <row r="169" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B169">
         <v>7990272</v>
@@ -7743,7 +7749,7 @@
         <v>7990272364</v>
       </c>
       <c r="D169" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E169" s="2">
         <v>45567</v>
@@ -7769,7 +7775,7 @@
     </row>
     <row r="170" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B170">
         <v>8008120</v>
@@ -7778,7 +7784,7 @@
         <v>8008120139</v>
       </c>
       <c r="D170" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E170" s="2">
         <v>45567</v>
@@ -7810,7 +7816,7 @@
     </row>
     <row r="171" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B171">
         <v>8008461</v>
@@ -7819,7 +7825,7 @@
         <v>8008461142</v>
       </c>
       <c r="D171" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E171" s="2">
         <v>45567</v>
@@ -7851,7 +7857,7 @@
     </row>
     <row r="172" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B172">
         <v>8029189</v>
@@ -7860,7 +7866,7 @@
         <v>8029189357</v>
       </c>
       <c r="D172" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E172" s="2">
         <v>45568</v>
@@ -7886,7 +7892,7 @@
     </row>
     <row r="173" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B173">
         <v>8035599</v>
@@ -7895,7 +7901,7 @@
         <v>8035599325</v>
       </c>
       <c r="D173" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E173" s="2">
         <v>45568</v>
@@ -7921,7 +7927,7 @@
     </row>
     <row r="174" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B174">
         <v>8050220</v>
@@ -7930,7 +7936,7 @@
         <v>8050220303</v>
       </c>
       <c r="D174" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E174" s="2">
         <v>45569</v>
@@ -7956,7 +7962,7 @@
     </row>
     <row r="175" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B175">
         <v>8054344</v>
@@ -7965,7 +7971,7 @@
         <v>8054344338</v>
       </c>
       <c r="D175" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E175" s="2">
         <v>45569</v>
@@ -7991,7 +7997,7 @@
     </row>
     <row r="176" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B176">
         <v>8059610</v>
@@ -8000,7 +8006,7 @@
         <v>8059610335</v>
       </c>
       <c r="D176" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E176" s="2">
         <v>45569</v>
@@ -8026,7 +8032,7 @@
     </row>
     <row r="177" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B177">
         <v>8061060</v>
@@ -8035,7 +8041,7 @@
         <v>8061060353</v>
       </c>
       <c r="D177" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E177" s="2">
         <v>45569</v>
@@ -8061,7 +8067,7 @@
     </row>
     <row r="178" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B178">
         <v>8068304</v>
@@ -8070,7 +8076,7 @@
         <v>8068304354</v>
       </c>
       <c r="D178" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E178" s="2">
         <v>45569</v>
@@ -8096,7 +8102,7 @@
     </row>
     <row r="179" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B179">
         <v>8097633</v>
@@ -8105,7 +8111,7 @@
         <v>8097633351</v>
       </c>
       <c r="D179" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E179" s="2">
         <v>45572</v>
@@ -8131,7 +8137,7 @@
     </row>
     <row r="180" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B180">
         <v>8116492</v>
@@ -8140,7 +8146,7 @@
         <v>8116492108</v>
       </c>
       <c r="D180" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E180" s="2">
         <v>45572</v>
@@ -8172,7 +8178,7 @@
     </row>
     <row r="181" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B181">
         <v>8116546</v>
@@ -8181,7 +8187,7 @@
         <v>8116546156</v>
       </c>
       <c r="D181" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E181" s="2">
         <v>45572</v>
@@ -8213,7 +8219,7 @@
     </row>
     <row r="182" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B182">
         <v>8132073</v>
@@ -8222,7 +8228,7 @@
         <v>8132073310</v>
       </c>
       <c r="D182" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E182" s="2">
         <v>45573</v>
@@ -8254,7 +8260,7 @@
     </row>
     <row r="183" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B183">
         <v>8132753</v>
@@ -8263,7 +8269,7 @@
         <v>8132753110</v>
       </c>
       <c r="D183" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E183" s="2">
         <v>45573</v>
@@ -8295,7 +8301,7 @@
     </row>
     <row r="184" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B184">
         <v>8132973</v>
@@ -8304,7 +8310,7 @@
         <v>8132973161</v>
       </c>
       <c r="D184" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E184" s="2">
         <v>45573</v>
@@ -8336,7 +8342,7 @@
     </row>
     <row r="185" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B185">
         <v>8133324</v>
@@ -8345,7 +8351,7 @@
         <v>8133324300</v>
       </c>
       <c r="D185" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E185" s="2">
         <v>45573</v>
@@ -8371,7 +8377,7 @@
     </row>
     <row r="186" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B186">
         <v>8150286</v>
@@ -8380,7 +8386,7 @@
         <v>8150286100</v>
       </c>
       <c r="D186" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E186" s="2">
         <v>45573</v>
@@ -8412,7 +8418,7 @@
     </row>
     <row r="187" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B187">
         <v>8150746</v>
@@ -8421,7 +8427,7 @@
         <v>8150746198</v>
       </c>
       <c r="D187" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E187" s="2">
         <v>45573</v>
@@ -8453,7 +8459,7 @@
     </row>
     <row r="188" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B188">
         <v>8151059</v>
@@ -8462,7 +8468,7 @@
         <v>8151059148</v>
       </c>
       <c r="D188" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E188" s="2">
         <v>45573</v>
@@ -8494,7 +8500,7 @@
     </row>
     <row r="189" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B189">
         <v>8151502</v>
@@ -8503,7 +8509,7 @@
         <v>8151502150</v>
       </c>
       <c r="D189" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E189" s="2">
         <v>45573</v>
@@ -8535,7 +8541,7 @@
     </row>
     <row r="190" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B190">
         <v>8152141</v>
@@ -8544,7 +8550,7 @@
         <v>8152141126</v>
       </c>
       <c r="D190" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E190" s="2">
         <v>45573</v>
@@ -8576,7 +8582,7 @@
     </row>
     <row r="191" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B191">
         <v>8183340</v>
@@ -8585,7 +8591,7 @@
         <v>8183340382</v>
       </c>
       <c r="D191" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E191" s="2">
         <v>45574</v>
@@ -8611,7 +8617,7 @@
     </row>
     <row r="192" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B192">
         <v>8183970</v>
@@ -8620,7 +8626,7 @@
         <v>8183970323</v>
       </c>
       <c r="D192" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E192" s="2">
         <v>45574</v>
@@ -8646,7 +8652,7 @@
     </row>
     <row r="193" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B193">
         <v>8184825</v>
@@ -8655,7 +8661,7 @@
         <v>8184825342</v>
       </c>
       <c r="D193" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E193" s="2">
         <v>45574</v>
@@ -8681,7 +8687,7 @@
     </row>
     <row r="194" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B194">
         <v>8185142</v>
@@ -8690,7 +8696,7 @@
         <v>8185142111</v>
       </c>
       <c r="D194" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E194" s="2">
         <v>45574</v>
@@ -8722,7 +8728,7 @@
     </row>
     <row r="195" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B195">
         <v>8185893</v>
@@ -8731,7 +8737,7 @@
         <v>8185893397</v>
       </c>
       <c r="D195" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E195" s="2">
         <v>45574</v>
@@ -8757,7 +8763,7 @@
     </row>
     <row r="196" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B196">
         <v>8186311</v>
@@ -8766,7 +8772,7 @@
         <v>8186311171</v>
       </c>
       <c r="D196" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E196" s="2">
         <v>45574</v>
@@ -8798,7 +8804,7 @@
     </row>
     <row r="197" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B197">
         <v>8209140</v>
@@ -8807,7 +8813,7 @@
         <v>8209140327</v>
       </c>
       <c r="D197" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E197" s="2">
         <v>45575</v>
@@ -8833,7 +8839,7 @@
     </row>
     <row r="198" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B198">
         <v>8255594</v>
@@ -8842,7 +8848,7 @@
         <v>8255594333</v>
       </c>
       <c r="D198" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E198" s="2">
         <v>45576</v>
@@ -8868,13 +8874,13 @@
     </row>
     <row r="199" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B199">
         <v>8256911</v>
       </c>
       <c r="D199" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="E199" s="2">
         <v>45576</v>

</xml_diff>

<commit_message>
execução do preenchimento do n° da carterinha para a confirmação do atendimento
</commit_message>
<xml_diff>
--- a/BASE_GUIAS_IPASGO_10-2024tTEST.xlsx
+++ b/BASE_GUIAS_IPASGO_10-2024tTEST.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="BaseSADT" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BaseSADT" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -938,10 +938,37 @@
       <c r="M10" t="n">
         <v>1</v>
       </c>
-      <c r="N10" t="inlineStr"/>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Erro no campo 'numeroDaCarteiraConfirmacao': Message: 
+Stacktrace:
+	GetHandleVerifier [0x00007FF6955C6CB5+28821]
+	(No symbol) [0x00007FF695533840]
+	(No symbol) [0x00007FF6953D578A]
+	(No symbol) [0x00007FF6954291BE]
+	(No symbol) [0x00007FF6954294AC]
+	(No symbol) [0x00007FF695472647]
+	(No symbol) [0x00007FF69544F33F]
+	(No symbol) [0x00007FF69546F412]
+	(No symbol) [0x00007FF69544F0A3]
+	(No symbol) [0x00007FF69541A778]
+	(No symbol) [0x00007FF69541B8E1]
+	GetHandleVerifier [0x00007FF6958FFCAD+3408013]
+	GetHandleVerifier [0x00007FF69591741F+3504127]
+	GetHandleVerifier [0x00007FF69590B5FD+3455453]
+	GetHandleVerifier [0x00007FF69568BDBB+835995]
+	(No symbol) [0x00007FF69553EB5F]
+	(No symbol) [0x00007FF69553A814]
+	(No symbol) [0x00007FF69553A9AD]
+	(No symbol) [0x00007FF69552A199]
+	BaseThreadInitThunk [0x00007FFB72B3259D+29]
+	RtlUserThreadStart [0x00007FFB739AAF38+40]
+</t>
+        </is>
+      </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Confirmado 17/10/2024; Confirmado 17/10/2024; Confirmado 31/10/2024; Confirmado 31/10/2024; Não confirmado; Não confirmado; Não confirmado; Não confirmado</t>
+          <t>Confirmado 17/10/2024; Confirmado 17/10/2024; Confirmado 31/10/2024; Confirmado 31/10/2024; Confirmado 21/11/2024; Confirmado 21/11/2024; Não confirmado; Não confirmado</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
finalizando a implementação da função Clicar_confirmar_procedimento(self), só faltando mudar a lógica da quantidade de confirmações.
</commit_message>
<xml_diff>
--- a/BASE_GUIAS_IPASGO_10-2024tTEST.xlsx
+++ b/BASE_GUIAS_IPASGO_10-2024tTEST.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BaseSADT" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="BaseSADT" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -942,27 +942,27 @@
         <is>
           <t xml:space="preserve">Erro no campo 'numeroDaCarteiraConfirmacao': Message: 
 Stacktrace:
-	GetHandleVerifier [0x00007FF6955C6CB5+28821]
-	(No symbol) [0x00007FF695533840]
-	(No symbol) [0x00007FF6953D578A]
-	(No symbol) [0x00007FF6954291BE]
-	(No symbol) [0x00007FF6954294AC]
-	(No symbol) [0x00007FF695472647]
-	(No symbol) [0x00007FF69544F33F]
-	(No symbol) [0x00007FF69546F412]
-	(No symbol) [0x00007FF69544F0A3]
-	(No symbol) [0x00007FF69541A778]
-	(No symbol) [0x00007FF69541B8E1]
-	GetHandleVerifier [0x00007FF6958FFCAD+3408013]
-	GetHandleVerifier [0x00007FF69591741F+3504127]
-	GetHandleVerifier [0x00007FF69590B5FD+3455453]
-	GetHandleVerifier [0x00007FF69568BDBB+835995]
-	(No symbol) [0x00007FF69553EB5F]
-	(No symbol) [0x00007FF69553A814]
-	(No symbol) [0x00007FF69553A9AD]
-	(No symbol) [0x00007FF69552A199]
-	BaseThreadInitThunk [0x00007FFB72B3259D+29]
-	RtlUserThreadStart [0x00007FFB739AAF38+40]
+	GetHandleVerifier [0x00007FF7D36B6CB5+28821]
+	(No symbol) [0x00007FF7D3623840]
+	(No symbol) [0x00007FF7D34C578A]
+	(No symbol) [0x00007FF7D35191BE]
+	(No symbol) [0x00007FF7D35194AC]
+	(No symbol) [0x00007FF7D3562647]
+	(No symbol) [0x00007FF7D353F33F]
+	(No symbol) [0x00007FF7D355F412]
+	(No symbol) [0x00007FF7D353F0A3]
+	(No symbol) [0x00007FF7D350A778]
+	(No symbol) [0x00007FF7D350B8E1]
+	GetHandleVerifier [0x00007FF7D39EFCAD+3408013]
+	GetHandleVerifier [0x00007FF7D3A0741F+3504127]
+	GetHandleVerifier [0x00007FF7D39FB5FD+3455453]
+	GetHandleVerifier [0x00007FF7D377BDBB+835995]
+	(No symbol) [0x00007FF7D362EB5F]
+	(No symbol) [0x00007FF7D362A814]
+	(No symbol) [0x00007FF7D362A9AD]
+	(No symbol) [0x00007FF7D361A199]
+	BaseThreadInitThunk [0x00007FFB5B20259D+29]
+	RtlUserThreadStart [0x00007FFB5C2CAF38+40]
 </t>
         </is>
       </c>

</xml_diff>

<commit_message>
atualizando ambas as versões de código, para a execução mais recente. Faltando apenas para ambas as funções adicionar a lógica de execução e alterar o funcionamento da função confirmar_datas
</commit_message>
<xml_diff>
--- a/BASE_GUIAS_IPASGO_10-2024tTEST.xlsx
+++ b/BASE_GUIAS_IPASGO_10-2024tTEST.xlsx
@@ -940,29 +940,7 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Erro no campo 'numeroDaCarteiraConfirmacao': Message: 
-Stacktrace:
-	GetHandleVerifier [0x00007FF7D36B6CB5+28821]
-	(No symbol) [0x00007FF7D3623840]
-	(No symbol) [0x00007FF7D34C578A]
-	(No symbol) [0x00007FF7D35191BE]
-	(No symbol) [0x00007FF7D35194AC]
-	(No symbol) [0x00007FF7D3562647]
-	(No symbol) [0x00007FF7D353F33F]
-	(No symbol) [0x00007FF7D355F412]
-	(No symbol) [0x00007FF7D353F0A3]
-	(No symbol) [0x00007FF7D350A778]
-	(No symbol) [0x00007FF7D350B8E1]
-	GetHandleVerifier [0x00007FF7D39EFCAD+3408013]
-	GetHandleVerifier [0x00007FF7D3A0741F+3504127]
-	GetHandleVerifier [0x00007FF7D39FB5FD+3455453]
-	GetHandleVerifier [0x00007FF7D377BDBB+835995]
-	(No symbol) [0x00007FF7D362EB5F]
-	(No symbol) [0x00007FF7D362A814]
-	(No symbol) [0x00007FF7D362A9AD]
-	(No symbol) [0x00007FF7D361A199]
-	BaseThreadInitThunk [0x00007FFB5B20259D+29]
-	RtlUserThreadStart [0x00007FFB5C2CAF38+40]
+          <t xml:space="preserve">Message: 
 </t>
         </is>
       </c>

</xml_diff>

<commit_message>
atualiando a versão l[ógica do código
</commit_message>
<xml_diff>
--- a/BASE_GUIAS_IPASGO_10-2024tTEST.xlsx
+++ b/BASE_GUIAS_IPASGO_10-2024tTEST.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O199"/>
+  <dimension ref="A1:O201"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9751,6 +9751,80 @@
       <c r="N199" t="inlineStr"/>
       <c r="O199" t="inlineStr"/>
     </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>ARTHUR SILVA PIRES</t>
+        </is>
+      </c>
+      <c r="B200" t="n">
+        <v>8921306</v>
+      </c>
+      <c r="C200" t="inlineStr"/>
+      <c r="D200" t="inlineStr">
+        <is>
+          <t>Autorizado</t>
+        </is>
+      </c>
+      <c r="E200" t="inlineStr"/>
+      <c r="F200" t="inlineStr"/>
+      <c r="G200" t="inlineStr"/>
+      <c r="H200" t="inlineStr"/>
+      <c r="I200" t="inlineStr"/>
+      <c r="J200" t="n">
+        <v>667325484</v>
+      </c>
+      <c r="K200" t="inlineStr"/>
+      <c r="L200" t="n">
+        <v>5</v>
+      </c>
+      <c r="M200" t="n">
+        <v>1</v>
+      </c>
+      <c r="N200" t="inlineStr"/>
+      <c r="O200" t="inlineStr">
+        <is>
+          <t>Confirmado 18/11/2024; Não confirmado; Não confirmado; Não confirmado; Não confirmado</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>LUI FERNANDO LOVO T. NETO</t>
+        </is>
+      </c>
+      <c r="B201" t="n">
+        <v>8921542</v>
+      </c>
+      <c r="C201" t="inlineStr"/>
+      <c r="D201" t="inlineStr">
+        <is>
+          <t>Autorizado</t>
+        </is>
+      </c>
+      <c r="E201" t="inlineStr"/>
+      <c r="F201" t="inlineStr"/>
+      <c r="G201" t="inlineStr"/>
+      <c r="H201" t="inlineStr"/>
+      <c r="I201" t="inlineStr"/>
+      <c r="J201" t="n">
+        <v>667182225</v>
+      </c>
+      <c r="K201" t="inlineStr"/>
+      <c r="L201" t="n">
+        <v>5</v>
+      </c>
+      <c r="M201" t="n">
+        <v>1</v>
+      </c>
+      <c r="N201" t="inlineStr"/>
+      <c r="O201" t="inlineStr">
+        <is>
+          <t>Confirmado 25/11/2024; Não confirmado</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>